<commit_message>
Updated pom.xml file and TestNG some script changes as per latest selenium changes related implicit waits
</commit_message>
<xml_diff>
--- a/src/com/testdata/From.xlsx
+++ b/src/com/testdata/From.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -32,9 +32,6 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ravi</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t xml:space="preserve">1234qwer</t>
   </si>
   <si>
-    <t xml:space="preserve">Pass</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tom</t>
   </si>
   <si>
@@ -63,6 +57,15 @@
   </si>
   <si>
     <t xml:space="preserve">9012opas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test4@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4572jhu</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,12 +126,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF969696"/>
-        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -174,11 +171,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,7 +433,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -444,66 +441,66 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16381" min="16381" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16382" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -511,6 +508,7 @@
     <hyperlink ref="B2" r:id="rId1" display="test1@gmail.com"/>
     <hyperlink ref="B3" r:id="rId2" display="test2@gmail.com"/>
     <hyperlink ref="B4" r:id="rId3" display="test3@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId4" display="test4@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>